<commit_message>
Unit Test for Excel Read/Write
</commit_message>
<xml_diff>
--- a/Ginger/Unit Tests/TestResources/EXCELS/TestExcel.xlsx
+++ b/Ginger/Unit Tests/TestResources/EXCELS/TestExcel.xlsx
@@ -19,12 +19,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -47,6 +41,12 @@
   </si>
   <si>
     <t>jadhav</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -398,44 +398,44 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>